<commit_message>
Changed budget parameters and capacity tolerance parameters
</commit_message>
<xml_diff>
--- a/analysis/new.batch.parameters.xlsx
+++ b/analysis/new.batch.parameters.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t xml:space="preserve">instance</t>
   </si>
@@ -38,178 +38,190 @@
     <t xml:space="preserve">tot_edges_installed</t>
   </si>
   <si>
+    <t xml:space="preserve">average.edge.capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">line_establish_capacity_coef_scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">line_upgrade_capacity_coef_scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dump_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tot.demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tot_potential_edges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">line_establish_cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">line_upgrade_cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max.expanse</t>
+  </si>
+  <si>
     <t xml:space="preserve">budget.constraint</t>
   </si>
   <si>
-    <t xml:space="preserve">average.edge.capacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">line_establish_capacity_coef_scale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">line_upgrade_capacity_coef_scale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dump_file</t>
-  </si>
-  <si>
     <t xml:space="preserve">runcommand</t>
   </si>
   <si>
-    <t xml:space="preserve">tot.demand</t>
-  </si>
-  <si>
     <t xml:space="preserve">robustness_heuristic_upper_bound.py</t>
   </si>
   <si>
-    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance30 --budget 50.06 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 11.0487804878049 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 22.0975609756098 --dump_file 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance57 --budget 115.22 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 23.8589743589744 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 47.7179487179487 --dump_file 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance118 --budget 1970.03 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 50.2877094972067 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 100.575418994413 --dump_file 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance300 --budget 5260.02 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 143.034229828851 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 286.068459657702 --dump_file 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance30 --budget 48.248 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance57 --budget 107.776 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance118 --budget 1934.024 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance300 --budget 5026.016 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance30 --budget 59.12 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 11.0487804878049 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 22.0975609756098 --dump_file 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance57 --budget 152.44 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 23.8589743589744 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 47.7179487179487 --dump_file 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance118 --budget 2150.06 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 50.2877094972067 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 100.575418994413 --dump_file 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance300 --budget 6430.04 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 143.034229828851 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 286.068459657702 --dump_file 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance30 --budget 55.496 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance57 --budget 137.552 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance118 --budget 2078.048 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance300 --budget 5962.032 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 16</t>
+    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance30 --budget 20.4698048780488 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance57 --budget 80.5526538461538 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance118 --budget 515.942162011173 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance300 --budget 2693.88209046455 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance30 --budget 22.9226341463415 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance57 --budget 91.0744615384615 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance118 --budget 566.933899441341 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance300 --budget 3026.43667481663 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance30 --budget 34.1163414634146 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance57 --budget 134.254423076923 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance118 --budget 859.903603351955 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance300 --budget 4489.80348410758 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance30 --budget 38.2043902439024 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance57 --budget 151.790769230769 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance118 --budget 944.889832402235 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance300 --budget 5044.06112469438 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 16</t>
   </si>
   <si>
     <t xml:space="preserve">main_program.py</t>
   </si>
   <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance30 --budget 50.06 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 11.0487804878049 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 22.0975609756098 --dump_file 17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance57 --budget 115.22 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 23.8589743589744 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 47.7179487179487 --dump_file 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance118 --budget 1970.03 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 50.2877094972067 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 100.575418994413 --dump_file 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance300 --budget 5260.02 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 143.034229828851 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 286.068459657702 --dump_file 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance30 --budget 48.248 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance57 --budget 107.776 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance118 --budget 1934.024 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance300 --budget 5026.016 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance30 --budget 59.12 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 11.0487804878049 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 22.0975609756098 --dump_file 25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance57 --budget 152.44 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 23.8589743589744 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 47.7179487179487 --dump_file 26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance118 --budget 2150.06 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 50.2877094972067 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 100.575418994413 --dump_file 27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance300 --budget 6430.04 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 143.034229828851 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 286.068459657702 --dump_file 28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance30 --budget 55.496 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance57 --budget 137.552 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance118 --budget 2078.048 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance300 --budget 5962.032 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 32</t>
+    <t xml:space="preserve">python main_program.py --instance_location instance30 --budget 20.4698048780488 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --instance_location instance57 --budget 80.5526538461538 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --instance_location instance118 --budget 515.942162011173 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --instance_location instance300 --budget 2693.88209046455 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --instance_location instance30 --budget 22.9226341463415 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --instance_location instance57 --budget 91.0744615384615 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --instance_location instance118 --budget 566.933899441341 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --instance_location instance300 --budget 3026.43667481663 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --instance_location instance30 --budget 34.1163414634146 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --instance_location instance57 --budget 134.254423076923 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --instance_location instance118 --budget 859.903603351955 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --instance_location instance300 --budget 4489.80348410758 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --instance_location instance30 --budget 38.2043902439024 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --instance_location instance57 --budget 151.790769230769 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --instance_location instance118 --budget 944.889832402235 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --instance_location instance300 --budget 5044.06112469438 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 32</t>
   </si>
   <si>
     <t xml:space="preserve">main_program_one_depth_cascade.py</t>
   </si>
   <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance30 --budget 50.06 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 11.0487804878049 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 22.0975609756098 --dump_file 33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance57 --budget 115.22 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 23.8589743589744 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 47.7179487179487 --dump_file 34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance118 --budget 1970.03 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 50.2877094972067 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 100.575418994413 --dump_file 35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance300 --budget 5260.02 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 143.034229828851 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 286.068459657702 --dump_file 36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance30 --budget 48.248 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance57 --budget 107.776 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance118 --budget 1934.024 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance300 --budget 5026.016 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance30 --budget 59.12 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 11.0487804878049 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 22.0975609756098 --dump_file 41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance57 --budget 152.44 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 23.8589743589744 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 47.7179487179487 --dump_file 42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance118 --budget 2150.06 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 50.2877094972067 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 100.575418994413 --dump_file 43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance300 --budget 6430.04 --load_capacity_factor 1 --line_upgrade_capacity_coef_scale 143.034229828851 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 286.068459657702 --dump_file 44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance30 --budget 55.496 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance57 --budget 137.552 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance118 --budget 2078.048 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance300 --budget 5962.032 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 48</t>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance30 --budget 20.4698048780488 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance57 --budget 80.5526538461538 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance118 --budget 515.942162011173 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance300 --budget 2693.88209046455 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance30 --budget 22.9226341463415 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance57 --budget 91.0744615384615 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance118 --budget 566.933899441341 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance300 --budget 3026.43667481663 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance30 --budget 34.1163414634146 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance57 --budget 134.254423076923 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance118 --budget 859.903603351955 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance300 --budget 4489.80348410758 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance30 --budget 38.2043902439024 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance57 --budget 151.790769230769 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance118 --budget 944.889832402235 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance300 --budget 5044.06112469438 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 48</t>
   </si>
 </sst>
 </file>
@@ -587,19 +599,31 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>30</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
@@ -608,31 +632,43 @@
         <v>0.1</v>
       </c>
       <c r="G2" t="n">
-        <v>906</v>
+        <v>634.2</v>
       </c>
       <c r="H2" t="n">
         <v>41</v>
       </c>
       <c r="I2" t="n">
-        <v>50.06</v>
+        <v>15.4682926829268</v>
       </c>
       <c r="J2" t="n">
-        <v>22.0975609756098</v>
+        <v>15.4682926829268</v>
       </c>
       <c r="K2" t="n">
-        <v>22.0975609756098</v>
+        <v>7.73414634146341</v>
       </c>
       <c r="L2" t="n">
-        <v>11.0487804878049</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
-        <v>16</v>
+        <v>189.2</v>
+      </c>
+      <c r="N2" t="n">
+        <v>11</v>
       </c>
       <c r="O2" t="n">
-        <v>189.2</v>
+        <v>2.54682926829268</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.773414634146341</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>68.2326829268293</v>
+      </c>
+      <c r="R2" t="n">
+        <v>20.4698048780488</v>
+      </c>
+      <c r="S2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -640,13 +676,13 @@
         <v>57</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
@@ -655,31 +691,43 @@
         <v>0.1</v>
       </c>
       <c r="G3" t="n">
-        <v>3722</v>
+        <v>2605.4</v>
       </c>
       <c r="H3" t="n">
         <v>78</v>
       </c>
       <c r="I3" t="n">
-        <v>115.22</v>
+        <v>33.4025641025641</v>
       </c>
       <c r="J3" t="n">
-        <v>47.7179487179487</v>
+        <v>33.4025641025641</v>
       </c>
       <c r="K3" t="n">
-        <v>47.7179487179487</v>
+        <v>16.701282051282</v>
       </c>
       <c r="L3" t="n">
-        <v>23.8589743589744</v>
+        <v>2</v>
       </c>
       <c r="M3" t="n">
-        <v>2</v>
-      </c>
-      <c r="N3" t="s">
-        <v>17</v>
+        <v>1250.8</v>
+      </c>
+      <c r="N3" t="n">
+        <v>23</v>
       </c>
       <c r="O3" t="n">
-        <v>1250.8</v>
+        <v>4.34025641025641</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1.67012820512821</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>268.508846153846</v>
+      </c>
+      <c r="R3" t="n">
+        <v>80.5526538461538</v>
+      </c>
+      <c r="S3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4">
@@ -687,13 +735,13 @@
         <v>118</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E4" t="n">
         <v>10</v>
@@ -702,31 +750,43 @@
         <v>0.1</v>
       </c>
       <c r="G4" t="n">
-        <v>18003</v>
+        <v>12602.1</v>
       </c>
       <c r="H4" t="n">
         <v>179</v>
       </c>
       <c r="I4" t="n">
-        <v>1970.03</v>
+        <v>70.4027932960894</v>
       </c>
       <c r="J4" t="n">
-        <v>100.575418994413</v>
+        <v>70.4027932960894</v>
       </c>
       <c r="K4" t="n">
-        <v>100.575418994413</v>
+        <v>35.2013966480447</v>
       </c>
       <c r="L4" t="n">
-        <v>50.2877094972067</v>
+        <v>3</v>
       </c>
       <c r="M4" t="n">
-        <v>3</v>
-      </c>
-      <c r="N4" t="s">
-        <v>18</v>
+        <v>4242</v>
+      </c>
+      <c r="N4" t="n">
+        <v>53</v>
       </c>
       <c r="O4" t="n">
-        <v>4242</v>
+        <v>17.0402793296089</v>
+      </c>
+      <c r="P4" t="n">
+        <v>3.52013966480447</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>1719.80720670391</v>
+      </c>
+      <c r="R4" t="n">
+        <v>515.942162011173</v>
+      </c>
+      <c r="S4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5">
@@ -734,13 +794,13 @@
         <v>300</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E5" t="n">
         <v>10</v>
@@ -749,31 +809,43 @@
         <v>0.1</v>
       </c>
       <c r="G5" t="n">
-        <v>117002</v>
+        <v>81901.4</v>
       </c>
       <c r="H5" t="n">
         <v>409</v>
       </c>
       <c r="I5" t="n">
-        <v>5260.02</v>
+        <v>200.247921760391</v>
       </c>
       <c r="J5" t="n">
-        <v>286.068459657702</v>
+        <v>200.247921760391</v>
       </c>
       <c r="K5" t="n">
-        <v>286.068459657702</v>
+        <v>100.123960880196</v>
       </c>
       <c r="L5" t="n">
-        <v>143.034229828851</v>
+        <v>4</v>
       </c>
       <c r="M5" t="n">
-        <v>4</v>
-      </c>
-      <c r="N5" t="s">
-        <v>19</v>
+        <v>23847.65</v>
+      </c>
+      <c r="N5" t="n">
+        <v>122</v>
       </c>
       <c r="O5" t="n">
-        <v>23847.65</v>
+        <v>30.0247921760391</v>
+      </c>
+      <c r="P5" t="n">
+        <v>10.0123960880196</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>8979.60696821516</v>
+      </c>
+      <c r="R5" t="n">
+        <v>2693.88209046455</v>
+      </c>
+      <c r="S5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6">
@@ -784,10 +856,10 @@
         <v>0.8</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
@@ -802,25 +874,37 @@
         <v>41</v>
       </c>
       <c r="I6" t="n">
-        <v>48.248</v>
+        <v>17.6780487804878</v>
       </c>
       <c r="J6" t="n">
         <v>17.6780487804878</v>
       </c>
       <c r="K6" t="n">
-        <v>17.6780487804878</v>
+        <v>8.8390243902439</v>
       </c>
       <c r="L6" t="n">
-        <v>8.8390243902439</v>
+        <v>5</v>
       </c>
       <c r="M6" t="n">
-        <v>5</v>
-      </c>
-      <c r="N6" t="s">
-        <v>20</v>
+        <v>189.2</v>
+      </c>
+      <c r="N6" t="n">
+        <v>11</v>
       </c>
       <c r="O6" t="n">
-        <v>189.2</v>
+        <v>2.76780487804878</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.88390243902439</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>76.4087804878049</v>
+      </c>
+      <c r="R6" t="n">
+        <v>22.9226341463415</v>
+      </c>
+      <c r="S6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7">
@@ -831,10 +915,10 @@
         <v>0.8</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -849,25 +933,37 @@
         <v>78</v>
       </c>
       <c r="I7" t="n">
-        <v>107.776</v>
+        <v>38.174358974359</v>
       </c>
       <c r="J7" t="n">
         <v>38.174358974359</v>
       </c>
       <c r="K7" t="n">
-        <v>38.174358974359</v>
+        <v>19.0871794871795</v>
       </c>
       <c r="L7" t="n">
-        <v>19.0871794871795</v>
+        <v>6</v>
       </c>
       <c r="M7" t="n">
-        <v>6</v>
-      </c>
-      <c r="N7" t="s">
-        <v>21</v>
+        <v>1250.8</v>
+      </c>
+      <c r="N7" t="n">
+        <v>23</v>
       </c>
       <c r="O7" t="n">
-        <v>1250.8</v>
+        <v>4.8174358974359</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1.90871794871795</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>303.581538461539</v>
+      </c>
+      <c r="R7" t="n">
+        <v>91.0744615384615</v>
+      </c>
+      <c r="S7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -878,10 +974,10 @@
         <v>0.8</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E8" t="n">
         <v>10</v>
@@ -896,25 +992,37 @@
         <v>179</v>
       </c>
       <c r="I8" t="n">
-        <v>1934.024</v>
+        <v>80.4603351955307</v>
       </c>
       <c r="J8" t="n">
         <v>80.4603351955307</v>
       </c>
       <c r="K8" t="n">
-        <v>80.4603351955307</v>
+        <v>40.2301675977654</v>
       </c>
       <c r="L8" t="n">
-        <v>40.2301675977654</v>
+        <v>7</v>
       </c>
       <c r="M8" t="n">
-        <v>7</v>
-      </c>
-      <c r="N8" t="s">
-        <v>22</v>
+        <v>4242</v>
+      </c>
+      <c r="N8" t="n">
+        <v>53</v>
       </c>
       <c r="O8" t="n">
-        <v>4242</v>
+        <v>18.0460335195531</v>
+      </c>
+      <c r="P8" t="n">
+        <v>4.02301675977654</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1889.77966480447</v>
+      </c>
+      <c r="R8" t="n">
+        <v>566.933899441341</v>
+      </c>
+      <c r="S8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9">
@@ -925,10 +1033,10 @@
         <v>0.8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E9" t="n">
         <v>10</v>
@@ -943,25 +1051,37 @@
         <v>409</v>
       </c>
       <c r="I9" t="n">
-        <v>5026.016</v>
+        <v>228.854767726161</v>
       </c>
       <c r="J9" t="n">
         <v>228.854767726161</v>
       </c>
       <c r="K9" t="n">
-        <v>228.854767726161</v>
+        <v>114.427383863081</v>
       </c>
       <c r="L9" t="n">
-        <v>114.427383863081</v>
+        <v>8</v>
       </c>
       <c r="M9" t="n">
-        <v>8</v>
-      </c>
-      <c r="N9" t="s">
-        <v>23</v>
+        <v>23847.65</v>
+      </c>
+      <c r="N9" t="n">
+        <v>122</v>
       </c>
       <c r="O9" t="n">
-        <v>23847.65</v>
+        <v>32.8854767726161</v>
+      </c>
+      <c r="P9" t="n">
+        <v>11.4427383863081</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>10088.1222493888</v>
+      </c>
+      <c r="R9" t="n">
+        <v>3026.43667481663</v>
+      </c>
+      <c r="S9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10">
@@ -969,13 +1089,13 @@
         <v>30</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
@@ -984,31 +1104,43 @@
         <v>0.1</v>
       </c>
       <c r="G10" t="n">
-        <v>906</v>
+        <v>634.2</v>
       </c>
       <c r="H10" t="n">
         <v>41</v>
       </c>
       <c r="I10" t="n">
-        <v>59.12</v>
+        <v>15.4682926829268</v>
       </c>
       <c r="J10" t="n">
-        <v>22.0975609756098</v>
+        <v>15.4682926829268</v>
       </c>
       <c r="K10" t="n">
-        <v>22.0975609756098</v>
+        <v>7.73414634146341</v>
       </c>
       <c r="L10" t="n">
-        <v>11.0487804878049</v>
+        <v>9</v>
       </c>
       <c r="M10" t="n">
-        <v>9</v>
-      </c>
-      <c r="N10" t="s">
-        <v>24</v>
+        <v>189.2</v>
+      </c>
+      <c r="N10" t="n">
+        <v>11</v>
       </c>
       <c r="O10" t="n">
-        <v>189.2</v>
+        <v>2.54682926829268</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.773414634146341</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>68.2326829268293</v>
+      </c>
+      <c r="R10" t="n">
+        <v>34.1163414634146</v>
+      </c>
+      <c r="S10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11">
@@ -1016,13 +1148,13 @@
         <v>57</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
@@ -1031,31 +1163,43 @@
         <v>0.1</v>
       </c>
       <c r="G11" t="n">
-        <v>3722</v>
+        <v>2605.4</v>
       </c>
       <c r="H11" t="n">
         <v>78</v>
       </c>
       <c r="I11" t="n">
-        <v>152.44</v>
+        <v>33.4025641025641</v>
       </c>
       <c r="J11" t="n">
-        <v>47.7179487179487</v>
+        <v>33.4025641025641</v>
       </c>
       <c r="K11" t="n">
-        <v>47.7179487179487</v>
+        <v>16.701282051282</v>
       </c>
       <c r="L11" t="n">
-        <v>23.8589743589744</v>
+        <v>10</v>
       </c>
       <c r="M11" t="n">
-        <v>10</v>
-      </c>
-      <c r="N11" t="s">
-        <v>25</v>
+        <v>1250.8</v>
+      </c>
+      <c r="N11" t="n">
+        <v>23</v>
       </c>
       <c r="O11" t="n">
-        <v>1250.8</v>
+        <v>4.34025641025641</v>
+      </c>
+      <c r="P11" t="n">
+        <v>1.67012820512821</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>268.508846153846</v>
+      </c>
+      <c r="R11" t="n">
+        <v>134.254423076923</v>
+      </c>
+      <c r="S11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12">
@@ -1063,13 +1207,13 @@
         <v>118</v>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E12" t="n">
         <v>10</v>
@@ -1078,31 +1222,43 @@
         <v>0.1</v>
       </c>
       <c r="G12" t="n">
-        <v>18003</v>
+        <v>12602.1</v>
       </c>
       <c r="H12" t="n">
         <v>179</v>
       </c>
       <c r="I12" t="n">
-        <v>2150.06</v>
+        <v>70.4027932960894</v>
       </c>
       <c r="J12" t="n">
-        <v>100.575418994413</v>
+        <v>70.4027932960894</v>
       </c>
       <c r="K12" t="n">
-        <v>100.575418994413</v>
+        <v>35.2013966480447</v>
       </c>
       <c r="L12" t="n">
-        <v>50.2877094972067</v>
+        <v>11</v>
       </c>
       <c r="M12" t="n">
-        <v>11</v>
-      </c>
-      <c r="N12" t="s">
-        <v>26</v>
+        <v>4242</v>
+      </c>
+      <c r="N12" t="n">
+        <v>53</v>
       </c>
       <c r="O12" t="n">
-        <v>4242</v>
+        <v>17.0402793296089</v>
+      </c>
+      <c r="P12" t="n">
+        <v>3.52013966480447</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>1719.80720670391</v>
+      </c>
+      <c r="R12" t="n">
+        <v>859.903603351955</v>
+      </c>
+      <c r="S12" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13">
@@ -1110,13 +1266,13 @@
         <v>300</v>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E13" t="n">
         <v>10</v>
@@ -1125,31 +1281,43 @@
         <v>0.1</v>
       </c>
       <c r="G13" t="n">
-        <v>117002</v>
+        <v>81901.4</v>
       </c>
       <c r="H13" t="n">
         <v>409</v>
       </c>
       <c r="I13" t="n">
-        <v>6430.04</v>
+        <v>200.247921760391</v>
       </c>
       <c r="J13" t="n">
-        <v>286.068459657702</v>
+        <v>200.247921760391</v>
       </c>
       <c r="K13" t="n">
-        <v>286.068459657702</v>
+        <v>100.123960880196</v>
       </c>
       <c r="L13" t="n">
-        <v>143.034229828851</v>
+        <v>12</v>
       </c>
       <c r="M13" t="n">
-        <v>12</v>
-      </c>
-      <c r="N13" t="s">
-        <v>27</v>
+        <v>23847.65</v>
+      </c>
+      <c r="N13" t="n">
+        <v>122</v>
       </c>
       <c r="O13" t="n">
-        <v>23847.65</v>
+        <v>30.0247921760391</v>
+      </c>
+      <c r="P13" t="n">
+        <v>10.0123960880196</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>8979.60696821516</v>
+      </c>
+      <c r="R13" t="n">
+        <v>4489.80348410758</v>
+      </c>
+      <c r="S13" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14">
@@ -1160,10 +1328,10 @@
         <v>0.8</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
@@ -1178,25 +1346,37 @@
         <v>41</v>
       </c>
       <c r="I14" t="n">
-        <v>55.496</v>
+        <v>17.6780487804878</v>
       </c>
       <c r="J14" t="n">
         <v>17.6780487804878</v>
       </c>
       <c r="K14" t="n">
-        <v>17.6780487804878</v>
+        <v>8.8390243902439</v>
       </c>
       <c r="L14" t="n">
-        <v>8.8390243902439</v>
+        <v>13</v>
       </c>
       <c r="M14" t="n">
-        <v>13</v>
-      </c>
-      <c r="N14" t="s">
-        <v>28</v>
+        <v>189.2</v>
+      </c>
+      <c r="N14" t="n">
+        <v>11</v>
       </c>
       <c r="O14" t="n">
-        <v>189.2</v>
+        <v>2.76780487804878</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.88390243902439</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>76.4087804878049</v>
+      </c>
+      <c r="R14" t="n">
+        <v>38.2043902439024</v>
+      </c>
+      <c r="S14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15">
@@ -1207,10 +1387,10 @@
         <v>0.8</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
@@ -1225,25 +1405,37 @@
         <v>78</v>
       </c>
       <c r="I15" t="n">
-        <v>137.552</v>
+        <v>38.174358974359</v>
       </c>
       <c r="J15" t="n">
         <v>38.174358974359</v>
       </c>
       <c r="K15" t="n">
-        <v>38.174358974359</v>
+        <v>19.0871794871795</v>
       </c>
       <c r="L15" t="n">
-        <v>19.0871794871795</v>
+        <v>14</v>
       </c>
       <c r="M15" t="n">
-        <v>14</v>
-      </c>
-      <c r="N15" t="s">
-        <v>29</v>
+        <v>1250.8</v>
+      </c>
+      <c r="N15" t="n">
+        <v>23</v>
       </c>
       <c r="O15" t="n">
-        <v>1250.8</v>
+        <v>4.8174358974359</v>
+      </c>
+      <c r="P15" t="n">
+        <v>1.90871794871795</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>303.581538461539</v>
+      </c>
+      <c r="R15" t="n">
+        <v>151.790769230769</v>
+      </c>
+      <c r="S15" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="16">
@@ -1254,10 +1446,10 @@
         <v>0.8</v>
       </c>
       <c r="C16" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E16" t="n">
         <v>10</v>
@@ -1272,25 +1464,37 @@
         <v>179</v>
       </c>
       <c r="I16" t="n">
-        <v>2078.048</v>
+        <v>80.4603351955307</v>
       </c>
       <c r="J16" t="n">
         <v>80.4603351955307</v>
       </c>
       <c r="K16" t="n">
-        <v>80.4603351955307</v>
+        <v>40.2301675977654</v>
       </c>
       <c r="L16" t="n">
-        <v>40.2301675977654</v>
+        <v>15</v>
       </c>
       <c r="M16" t="n">
-        <v>15</v>
-      </c>
-      <c r="N16" t="s">
-        <v>30</v>
+        <v>4242</v>
+      </c>
+      <c r="N16" t="n">
+        <v>53</v>
       </c>
       <c r="O16" t="n">
-        <v>4242</v>
+        <v>18.0460335195531</v>
+      </c>
+      <c r="P16" t="n">
+        <v>4.02301675977654</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>1889.77966480447</v>
+      </c>
+      <c r="R16" t="n">
+        <v>944.889832402235</v>
+      </c>
+      <c r="S16" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17">
@@ -1301,10 +1505,10 @@
         <v>0.8</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E17" t="n">
         <v>10</v>
@@ -1319,25 +1523,37 @@
         <v>409</v>
       </c>
       <c r="I17" t="n">
-        <v>5962.032</v>
+        <v>228.854767726161</v>
       </c>
       <c r="J17" t="n">
         <v>228.854767726161</v>
       </c>
       <c r="K17" t="n">
-        <v>228.854767726161</v>
+        <v>114.427383863081</v>
       </c>
       <c r="L17" t="n">
-        <v>114.427383863081</v>
+        <v>16</v>
       </c>
       <c r="M17" t="n">
-        <v>16</v>
-      </c>
-      <c r="N17" t="s">
-        <v>31</v>
+        <v>23847.65</v>
+      </c>
+      <c r="N17" t="n">
+        <v>122</v>
       </c>
       <c r="O17" t="n">
-        <v>23847.65</v>
+        <v>32.8854767726161</v>
+      </c>
+      <c r="P17" t="n">
+        <v>11.4427383863081</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>10088.1222493888</v>
+      </c>
+      <c r="R17" t="n">
+        <v>5044.06112469438</v>
+      </c>
+      <c r="S17" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="18">
@@ -1345,13 +1561,13 @@
         <v>30</v>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E18" t="n">
         <v>1</v>
@@ -1360,31 +1576,43 @@
         <v>0.1</v>
       </c>
       <c r="G18" t="n">
-        <v>906</v>
+        <v>634.2</v>
       </c>
       <c r="H18" t="n">
         <v>41</v>
       </c>
       <c r="I18" t="n">
-        <v>50.06</v>
+        <v>15.4682926829268</v>
       </c>
       <c r="J18" t="n">
-        <v>22.0975609756098</v>
+        <v>15.4682926829268</v>
       </c>
       <c r="K18" t="n">
-        <v>22.0975609756098</v>
+        <v>7.73414634146341</v>
       </c>
       <c r="L18" t="n">
-        <v>11.0487804878049</v>
+        <v>17</v>
       </c>
       <c r="M18" t="n">
-        <v>17</v>
-      </c>
-      <c r="N18" t="s">
-        <v>33</v>
+        <v>189.2</v>
+      </c>
+      <c r="N18" t="n">
+        <v>11</v>
       </c>
       <c r="O18" t="n">
-        <v>189.2</v>
+        <v>2.54682926829268</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.773414634146341</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>68.2326829268293</v>
+      </c>
+      <c r="R18" t="n">
+        <v>20.4698048780488</v>
+      </c>
+      <c r="S18" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19">
@@ -1392,13 +1620,13 @@
         <v>57</v>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
@@ -1407,31 +1635,43 @@
         <v>0.1</v>
       </c>
       <c r="G19" t="n">
-        <v>3722</v>
+        <v>2605.4</v>
       </c>
       <c r="H19" t="n">
         <v>78</v>
       </c>
       <c r="I19" t="n">
-        <v>115.22</v>
+        <v>33.4025641025641</v>
       </c>
       <c r="J19" t="n">
-        <v>47.7179487179487</v>
+        <v>33.4025641025641</v>
       </c>
       <c r="K19" t="n">
-        <v>47.7179487179487</v>
+        <v>16.701282051282</v>
       </c>
       <c r="L19" t="n">
-        <v>23.8589743589744</v>
+        <v>18</v>
       </c>
       <c r="M19" t="n">
-        <v>18</v>
-      </c>
-      <c r="N19" t="s">
-        <v>34</v>
+        <v>1250.8</v>
+      </c>
+      <c r="N19" t="n">
+        <v>23</v>
       </c>
       <c r="O19" t="n">
-        <v>1250.8</v>
+        <v>4.34025641025641</v>
+      </c>
+      <c r="P19" t="n">
+        <v>1.67012820512821</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>268.508846153846</v>
+      </c>
+      <c r="R19" t="n">
+        <v>80.5526538461538</v>
+      </c>
+      <c r="S19" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20">
@@ -1439,13 +1679,13 @@
         <v>118</v>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E20" t="n">
         <v>10</v>
@@ -1454,31 +1694,43 @@
         <v>0.1</v>
       </c>
       <c r="G20" t="n">
-        <v>18003</v>
+        <v>12602.1</v>
       </c>
       <c r="H20" t="n">
         <v>179</v>
       </c>
       <c r="I20" t="n">
-        <v>1970.03</v>
+        <v>70.4027932960894</v>
       </c>
       <c r="J20" t="n">
-        <v>100.575418994413</v>
+        <v>70.4027932960894</v>
       </c>
       <c r="K20" t="n">
-        <v>100.575418994413</v>
+        <v>35.2013966480447</v>
       </c>
       <c r="L20" t="n">
-        <v>50.2877094972067</v>
+        <v>19</v>
       </c>
       <c r="M20" t="n">
-        <v>19</v>
-      </c>
-      <c r="N20" t="s">
-        <v>35</v>
+        <v>4242</v>
+      </c>
+      <c r="N20" t="n">
+        <v>53</v>
       </c>
       <c r="O20" t="n">
-        <v>4242</v>
+        <v>17.0402793296089</v>
+      </c>
+      <c r="P20" t="n">
+        <v>3.52013966480447</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>1719.80720670391</v>
+      </c>
+      <c r="R20" t="n">
+        <v>515.942162011173</v>
+      </c>
+      <c r="S20" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="21">
@@ -1486,13 +1738,13 @@
         <v>300</v>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C21" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E21" t="n">
         <v>10</v>
@@ -1501,31 +1753,43 @@
         <v>0.1</v>
       </c>
       <c r="G21" t="n">
-        <v>117002</v>
+        <v>81901.4</v>
       </c>
       <c r="H21" t="n">
         <v>409</v>
       </c>
       <c r="I21" t="n">
-        <v>5260.02</v>
+        <v>200.247921760391</v>
       </c>
       <c r="J21" t="n">
-        <v>286.068459657702</v>
+        <v>200.247921760391</v>
       </c>
       <c r="K21" t="n">
-        <v>286.068459657702</v>
+        <v>100.123960880196</v>
       </c>
       <c r="L21" t="n">
-        <v>143.034229828851</v>
+        <v>20</v>
       </c>
       <c r="M21" t="n">
-        <v>20</v>
-      </c>
-      <c r="N21" t="s">
-        <v>36</v>
+        <v>23847.65</v>
+      </c>
+      <c r="N21" t="n">
+        <v>122</v>
       </c>
       <c r="O21" t="n">
-        <v>23847.65</v>
+        <v>30.0247921760391</v>
+      </c>
+      <c r="P21" t="n">
+        <v>10.0123960880196</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>8979.60696821516</v>
+      </c>
+      <c r="R21" t="n">
+        <v>2693.88209046455</v>
+      </c>
+      <c r="S21" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="22">
@@ -1536,10 +1800,10 @@
         <v>0.8</v>
       </c>
       <c r="C22" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E22" t="n">
         <v>1</v>
@@ -1554,25 +1818,37 @@
         <v>41</v>
       </c>
       <c r="I22" t="n">
-        <v>48.248</v>
+        <v>17.6780487804878</v>
       </c>
       <c r="J22" t="n">
         <v>17.6780487804878</v>
       </c>
       <c r="K22" t="n">
-        <v>17.6780487804878</v>
+        <v>8.8390243902439</v>
       </c>
       <c r="L22" t="n">
-        <v>8.8390243902439</v>
+        <v>21</v>
       </c>
       <c r="M22" t="n">
-        <v>21</v>
-      </c>
-      <c r="N22" t="s">
-        <v>37</v>
+        <v>189.2</v>
+      </c>
+      <c r="N22" t="n">
+        <v>11</v>
       </c>
       <c r="O22" t="n">
-        <v>189.2</v>
+        <v>2.76780487804878</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.88390243902439</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>76.4087804878049</v>
+      </c>
+      <c r="R22" t="n">
+        <v>22.9226341463415</v>
+      </c>
+      <c r="S22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="23">
@@ -1583,10 +1859,10 @@
         <v>0.8</v>
       </c>
       <c r="C23" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E23" t="n">
         <v>1</v>
@@ -1601,25 +1877,37 @@
         <v>78</v>
       </c>
       <c r="I23" t="n">
-        <v>107.776</v>
+        <v>38.174358974359</v>
       </c>
       <c r="J23" t="n">
         <v>38.174358974359</v>
       </c>
       <c r="K23" t="n">
-        <v>38.174358974359</v>
+        <v>19.0871794871795</v>
       </c>
       <c r="L23" t="n">
-        <v>19.0871794871795</v>
+        <v>22</v>
       </c>
       <c r="M23" t="n">
-        <v>22</v>
-      </c>
-      <c r="N23" t="s">
-        <v>38</v>
+        <v>1250.8</v>
+      </c>
+      <c r="N23" t="n">
+        <v>23</v>
       </c>
       <c r="O23" t="n">
-        <v>1250.8</v>
+        <v>4.8174358974359</v>
+      </c>
+      <c r="P23" t="n">
+        <v>1.90871794871795</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>303.581538461539</v>
+      </c>
+      <c r="R23" t="n">
+        <v>91.0744615384615</v>
+      </c>
+      <c r="S23" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="24">
@@ -1630,10 +1918,10 @@
         <v>0.8</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E24" t="n">
         <v>10</v>
@@ -1648,25 +1936,37 @@
         <v>179</v>
       </c>
       <c r="I24" t="n">
-        <v>1934.024</v>
+        <v>80.4603351955307</v>
       </c>
       <c r="J24" t="n">
         <v>80.4603351955307</v>
       </c>
       <c r="K24" t="n">
-        <v>80.4603351955307</v>
+        <v>40.2301675977654</v>
       </c>
       <c r="L24" t="n">
-        <v>40.2301675977654</v>
+        <v>23</v>
       </c>
       <c r="M24" t="n">
-        <v>23</v>
-      </c>
-      <c r="N24" t="s">
-        <v>39</v>
+        <v>4242</v>
+      </c>
+      <c r="N24" t="n">
+        <v>53</v>
       </c>
       <c r="O24" t="n">
-        <v>4242</v>
+        <v>18.0460335195531</v>
+      </c>
+      <c r="P24" t="n">
+        <v>4.02301675977654</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>1889.77966480447</v>
+      </c>
+      <c r="R24" t="n">
+        <v>566.933899441341</v>
+      </c>
+      <c r="S24" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="25">
@@ -1677,10 +1977,10 @@
         <v>0.8</v>
       </c>
       <c r="C25" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E25" t="n">
         <v>10</v>
@@ -1695,25 +1995,37 @@
         <v>409</v>
       </c>
       <c r="I25" t="n">
-        <v>5026.016</v>
+        <v>228.854767726161</v>
       </c>
       <c r="J25" t="n">
         <v>228.854767726161</v>
       </c>
       <c r="K25" t="n">
-        <v>228.854767726161</v>
+        <v>114.427383863081</v>
       </c>
       <c r="L25" t="n">
-        <v>114.427383863081</v>
+        <v>24</v>
       </c>
       <c r="M25" t="n">
-        <v>24</v>
-      </c>
-      <c r="N25" t="s">
-        <v>40</v>
+        <v>23847.65</v>
+      </c>
+      <c r="N25" t="n">
+        <v>122</v>
       </c>
       <c r="O25" t="n">
-        <v>23847.65</v>
+        <v>32.8854767726161</v>
+      </c>
+      <c r="P25" t="n">
+        <v>11.4427383863081</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>10088.1222493888</v>
+      </c>
+      <c r="R25" t="n">
+        <v>3026.43667481663</v>
+      </c>
+      <c r="S25" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="26">
@@ -1721,13 +2033,13 @@
         <v>30</v>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C26" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E26" t="n">
         <v>1</v>
@@ -1736,31 +2048,43 @@
         <v>0.1</v>
       </c>
       <c r="G26" t="n">
-        <v>906</v>
+        <v>634.2</v>
       </c>
       <c r="H26" t="n">
         <v>41</v>
       </c>
       <c r="I26" t="n">
-        <v>59.12</v>
+        <v>15.4682926829268</v>
       </c>
       <c r="J26" t="n">
-        <v>22.0975609756098</v>
+        <v>15.4682926829268</v>
       </c>
       <c r="K26" t="n">
-        <v>22.0975609756098</v>
+        <v>7.73414634146341</v>
       </c>
       <c r="L26" t="n">
-        <v>11.0487804878049</v>
+        <v>25</v>
       </c>
       <c r="M26" t="n">
-        <v>25</v>
-      </c>
-      <c r="N26" t="s">
-        <v>41</v>
+        <v>189.2</v>
+      </c>
+      <c r="N26" t="n">
+        <v>11</v>
       </c>
       <c r="O26" t="n">
-        <v>189.2</v>
+        <v>2.54682926829268</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0.773414634146341</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>68.2326829268293</v>
+      </c>
+      <c r="R26" t="n">
+        <v>34.1163414634146</v>
+      </c>
+      <c r="S26" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="27">
@@ -1768,13 +2092,13 @@
         <v>57</v>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C27" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D27" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E27" t="n">
         <v>1</v>
@@ -1783,31 +2107,43 @@
         <v>0.1</v>
       </c>
       <c r="G27" t="n">
-        <v>3722</v>
+        <v>2605.4</v>
       </c>
       <c r="H27" t="n">
         <v>78</v>
       </c>
       <c r="I27" t="n">
-        <v>152.44</v>
+        <v>33.4025641025641</v>
       </c>
       <c r="J27" t="n">
-        <v>47.7179487179487</v>
+        <v>33.4025641025641</v>
       </c>
       <c r="K27" t="n">
-        <v>47.7179487179487</v>
+        <v>16.701282051282</v>
       </c>
       <c r="L27" t="n">
-        <v>23.8589743589744</v>
+        <v>26</v>
       </c>
       <c r="M27" t="n">
-        <v>26</v>
-      </c>
-      <c r="N27" t="s">
-        <v>42</v>
+        <v>1250.8</v>
+      </c>
+      <c r="N27" t="n">
+        <v>23</v>
       </c>
       <c r="O27" t="n">
-        <v>1250.8</v>
+        <v>4.34025641025641</v>
+      </c>
+      <c r="P27" t="n">
+        <v>1.67012820512821</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>268.508846153846</v>
+      </c>
+      <c r="R27" t="n">
+        <v>134.254423076923</v>
+      </c>
+      <c r="S27" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="28">
@@ -1815,13 +2151,13 @@
         <v>118</v>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C28" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E28" t="n">
         <v>10</v>
@@ -1830,31 +2166,43 @@
         <v>0.1</v>
       </c>
       <c r="G28" t="n">
-        <v>18003</v>
+        <v>12602.1</v>
       </c>
       <c r="H28" t="n">
         <v>179</v>
       </c>
       <c r="I28" t="n">
-        <v>2150.06</v>
+        <v>70.4027932960894</v>
       </c>
       <c r="J28" t="n">
-        <v>100.575418994413</v>
+        <v>70.4027932960894</v>
       </c>
       <c r="K28" t="n">
-        <v>100.575418994413</v>
+        <v>35.2013966480447</v>
       </c>
       <c r="L28" t="n">
-        <v>50.2877094972067</v>
+        <v>27</v>
       </c>
       <c r="M28" t="n">
-        <v>27</v>
-      </c>
-      <c r="N28" t="s">
-        <v>43</v>
+        <v>4242</v>
+      </c>
+      <c r="N28" t="n">
+        <v>53</v>
       </c>
       <c r="O28" t="n">
-        <v>4242</v>
+        <v>17.0402793296089</v>
+      </c>
+      <c r="P28" t="n">
+        <v>3.52013966480447</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>1719.80720670391</v>
+      </c>
+      <c r="R28" t="n">
+        <v>859.903603351955</v>
+      </c>
+      <c r="S28" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="29">
@@ -1862,13 +2210,13 @@
         <v>300</v>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C29" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D29" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E29" t="n">
         <v>10</v>
@@ -1877,31 +2225,43 @@
         <v>0.1</v>
       </c>
       <c r="G29" t="n">
-        <v>117002</v>
+        <v>81901.4</v>
       </c>
       <c r="H29" t="n">
         <v>409</v>
       </c>
       <c r="I29" t="n">
-        <v>6430.04</v>
+        <v>200.247921760391</v>
       </c>
       <c r="J29" t="n">
-        <v>286.068459657702</v>
+        <v>200.247921760391</v>
       </c>
       <c r="K29" t="n">
-        <v>286.068459657702</v>
+        <v>100.123960880196</v>
       </c>
       <c r="L29" t="n">
-        <v>143.034229828851</v>
+        <v>28</v>
       </c>
       <c r="M29" t="n">
-        <v>28</v>
-      </c>
-      <c r="N29" t="s">
-        <v>44</v>
+        <v>23847.65</v>
+      </c>
+      <c r="N29" t="n">
+        <v>122</v>
       </c>
       <c r="O29" t="n">
-        <v>23847.65</v>
+        <v>30.0247921760391</v>
+      </c>
+      <c r="P29" t="n">
+        <v>10.0123960880196</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>8979.60696821516</v>
+      </c>
+      <c r="R29" t="n">
+        <v>4489.80348410758</v>
+      </c>
+      <c r="S29" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="30">
@@ -1912,10 +2272,10 @@
         <v>0.8</v>
       </c>
       <c r="C30" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>
@@ -1930,25 +2290,37 @@
         <v>41</v>
       </c>
       <c r="I30" t="n">
-        <v>55.496</v>
+        <v>17.6780487804878</v>
       </c>
       <c r="J30" t="n">
         <v>17.6780487804878</v>
       </c>
       <c r="K30" t="n">
-        <v>17.6780487804878</v>
+        <v>8.8390243902439</v>
       </c>
       <c r="L30" t="n">
-        <v>8.8390243902439</v>
+        <v>29</v>
       </c>
       <c r="M30" t="n">
-        <v>29</v>
-      </c>
-      <c r="N30" t="s">
-        <v>45</v>
+        <v>189.2</v>
+      </c>
+      <c r="N30" t="n">
+        <v>11</v>
       </c>
       <c r="O30" t="n">
-        <v>189.2</v>
+        <v>2.76780487804878</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0.88390243902439</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>76.4087804878049</v>
+      </c>
+      <c r="R30" t="n">
+        <v>38.2043902439024</v>
+      </c>
+      <c r="S30" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="31">
@@ -1959,10 +2331,10 @@
         <v>0.8</v>
       </c>
       <c r="C31" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D31" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E31" t="n">
         <v>1</v>
@@ -1977,25 +2349,37 @@
         <v>78</v>
       </c>
       <c r="I31" t="n">
-        <v>137.552</v>
+        <v>38.174358974359</v>
       </c>
       <c r="J31" t="n">
         <v>38.174358974359</v>
       </c>
       <c r="K31" t="n">
-        <v>38.174358974359</v>
+        <v>19.0871794871795</v>
       </c>
       <c r="L31" t="n">
-        <v>19.0871794871795</v>
+        <v>30</v>
       </c>
       <c r="M31" t="n">
-        <v>30</v>
-      </c>
-      <c r="N31" t="s">
-        <v>46</v>
+        <v>1250.8</v>
+      </c>
+      <c r="N31" t="n">
+        <v>23</v>
       </c>
       <c r="O31" t="n">
-        <v>1250.8</v>
+        <v>4.8174358974359</v>
+      </c>
+      <c r="P31" t="n">
+        <v>1.90871794871795</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>303.581538461539</v>
+      </c>
+      <c r="R31" t="n">
+        <v>151.790769230769</v>
+      </c>
+      <c r="S31" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="32">
@@ -2006,10 +2390,10 @@
         <v>0.8</v>
       </c>
       <c r="C32" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D32" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E32" t="n">
         <v>10</v>
@@ -2024,25 +2408,37 @@
         <v>179</v>
       </c>
       <c r="I32" t="n">
-        <v>2078.048</v>
+        <v>80.4603351955307</v>
       </c>
       <c r="J32" t="n">
         <v>80.4603351955307</v>
       </c>
       <c r="K32" t="n">
-        <v>80.4603351955307</v>
+        <v>40.2301675977654</v>
       </c>
       <c r="L32" t="n">
-        <v>40.2301675977654</v>
+        <v>31</v>
       </c>
       <c r="M32" t="n">
-        <v>31</v>
-      </c>
-      <c r="N32" t="s">
-        <v>47</v>
+        <v>4242</v>
+      </c>
+      <c r="N32" t="n">
+        <v>53</v>
       </c>
       <c r="O32" t="n">
-        <v>4242</v>
+        <v>18.0460335195531</v>
+      </c>
+      <c r="P32" t="n">
+        <v>4.02301675977654</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>1889.77966480447</v>
+      </c>
+      <c r="R32" t="n">
+        <v>944.889832402235</v>
+      </c>
+      <c r="S32" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="33">
@@ -2053,10 +2449,10 @@
         <v>0.8</v>
       </c>
       <c r="C33" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D33" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E33" t="n">
         <v>10</v>
@@ -2071,25 +2467,37 @@
         <v>409</v>
       </c>
       <c r="I33" t="n">
-        <v>5962.032</v>
+        <v>228.854767726161</v>
       </c>
       <c r="J33" t="n">
         <v>228.854767726161</v>
       </c>
       <c r="K33" t="n">
-        <v>228.854767726161</v>
+        <v>114.427383863081</v>
       </c>
       <c r="L33" t="n">
-        <v>114.427383863081</v>
+        <v>32</v>
       </c>
       <c r="M33" t="n">
-        <v>32</v>
-      </c>
-      <c r="N33" t="s">
-        <v>48</v>
+        <v>23847.65</v>
+      </c>
+      <c r="N33" t="n">
+        <v>122</v>
       </c>
       <c r="O33" t="n">
-        <v>23847.65</v>
+        <v>32.8854767726161</v>
+      </c>
+      <c r="P33" t="n">
+        <v>11.4427383863081</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>10088.1222493888</v>
+      </c>
+      <c r="R33" t="n">
+        <v>5044.06112469438</v>
+      </c>
+      <c r="S33" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="34">
@@ -2097,13 +2505,13 @@
         <v>30</v>
       </c>
       <c r="B34" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C34" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D34" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E34" t="n">
         <v>1</v>
@@ -2112,31 +2520,43 @@
         <v>0.1</v>
       </c>
       <c r="G34" t="n">
-        <v>906</v>
+        <v>634.2</v>
       </c>
       <c r="H34" t="n">
         <v>41</v>
       </c>
       <c r="I34" t="n">
-        <v>50.06</v>
+        <v>15.4682926829268</v>
       </c>
       <c r="J34" t="n">
-        <v>22.0975609756098</v>
+        <v>15.4682926829268</v>
       </c>
       <c r="K34" t="n">
-        <v>22.0975609756098</v>
+        <v>7.73414634146341</v>
       </c>
       <c r="L34" t="n">
-        <v>11.0487804878049</v>
+        <v>33</v>
       </c>
       <c r="M34" t="n">
-        <v>33</v>
-      </c>
-      <c r="N34" t="s">
-        <v>50</v>
+        <v>189.2</v>
+      </c>
+      <c r="N34" t="n">
+        <v>11</v>
       </c>
       <c r="O34" t="n">
-        <v>189.2</v>
+        <v>2.54682926829268</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0.773414634146341</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>68.2326829268293</v>
+      </c>
+      <c r="R34" t="n">
+        <v>20.4698048780488</v>
+      </c>
+      <c r="S34" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="35">
@@ -2144,13 +2564,13 @@
         <v>57</v>
       </c>
       <c r="B35" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C35" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D35" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E35" t="n">
         <v>1</v>
@@ -2159,31 +2579,43 @@
         <v>0.1</v>
       </c>
       <c r="G35" t="n">
-        <v>3722</v>
+        <v>2605.4</v>
       </c>
       <c r="H35" t="n">
         <v>78</v>
       </c>
       <c r="I35" t="n">
-        <v>115.22</v>
+        <v>33.4025641025641</v>
       </c>
       <c r="J35" t="n">
-        <v>47.7179487179487</v>
+        <v>33.4025641025641</v>
       </c>
       <c r="K35" t="n">
-        <v>47.7179487179487</v>
+        <v>16.701282051282</v>
       </c>
       <c r="L35" t="n">
-        <v>23.8589743589744</v>
+        <v>34</v>
       </c>
       <c r="M35" t="n">
-        <v>34</v>
-      </c>
-      <c r="N35" t="s">
-        <v>51</v>
+        <v>1250.8</v>
+      </c>
+      <c r="N35" t="n">
+        <v>23</v>
       </c>
       <c r="O35" t="n">
-        <v>1250.8</v>
+        <v>4.34025641025641</v>
+      </c>
+      <c r="P35" t="n">
+        <v>1.67012820512821</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>268.508846153846</v>
+      </c>
+      <c r="R35" t="n">
+        <v>80.5526538461538</v>
+      </c>
+      <c r="S35" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="36">
@@ -2191,13 +2623,13 @@
         <v>118</v>
       </c>
       <c r="B36" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C36" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D36" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E36" t="n">
         <v>10</v>
@@ -2206,31 +2638,43 @@
         <v>0.1</v>
       </c>
       <c r="G36" t="n">
-        <v>18003</v>
+        <v>12602.1</v>
       </c>
       <c r="H36" t="n">
         <v>179</v>
       </c>
       <c r="I36" t="n">
-        <v>1970.03</v>
+        <v>70.4027932960894</v>
       </c>
       <c r="J36" t="n">
-        <v>100.575418994413</v>
+        <v>70.4027932960894</v>
       </c>
       <c r="K36" t="n">
-        <v>100.575418994413</v>
+        <v>35.2013966480447</v>
       </c>
       <c r="L36" t="n">
-        <v>50.2877094972067</v>
+        <v>35</v>
       </c>
       <c r="M36" t="n">
-        <v>35</v>
-      </c>
-      <c r="N36" t="s">
-        <v>52</v>
+        <v>4242</v>
+      </c>
+      <c r="N36" t="n">
+        <v>53</v>
       </c>
       <c r="O36" t="n">
-        <v>4242</v>
+        <v>17.0402793296089</v>
+      </c>
+      <c r="P36" t="n">
+        <v>3.52013966480447</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>1719.80720670391</v>
+      </c>
+      <c r="R36" t="n">
+        <v>515.942162011173</v>
+      </c>
+      <c r="S36" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="37">
@@ -2238,13 +2682,13 @@
         <v>300</v>
       </c>
       <c r="B37" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C37" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D37" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E37" t="n">
         <v>10</v>
@@ -2253,31 +2697,43 @@
         <v>0.1</v>
       </c>
       <c r="G37" t="n">
-        <v>117002</v>
+        <v>81901.4</v>
       </c>
       <c r="H37" t="n">
         <v>409</v>
       </c>
       <c r="I37" t="n">
-        <v>5260.02</v>
+        <v>200.247921760391</v>
       </c>
       <c r="J37" t="n">
-        <v>286.068459657702</v>
+        <v>200.247921760391</v>
       </c>
       <c r="K37" t="n">
-        <v>286.068459657702</v>
+        <v>100.123960880196</v>
       </c>
       <c r="L37" t="n">
-        <v>143.034229828851</v>
+        <v>36</v>
       </c>
       <c r="M37" t="n">
-        <v>36</v>
-      </c>
-      <c r="N37" t="s">
-        <v>53</v>
+        <v>23847.65</v>
+      </c>
+      <c r="N37" t="n">
+        <v>122</v>
       </c>
       <c r="O37" t="n">
-        <v>23847.65</v>
+        <v>30.0247921760391</v>
+      </c>
+      <c r="P37" t="n">
+        <v>10.0123960880196</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>8979.60696821516</v>
+      </c>
+      <c r="R37" t="n">
+        <v>2693.88209046455</v>
+      </c>
+      <c r="S37" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="38">
@@ -2288,10 +2744,10 @@
         <v>0.8</v>
       </c>
       <c r="C38" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D38" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E38" t="n">
         <v>1</v>
@@ -2306,25 +2762,37 @@
         <v>41</v>
       </c>
       <c r="I38" t="n">
-        <v>48.248</v>
+        <v>17.6780487804878</v>
       </c>
       <c r="J38" t="n">
         <v>17.6780487804878</v>
       </c>
       <c r="K38" t="n">
-        <v>17.6780487804878</v>
+        <v>8.8390243902439</v>
       </c>
       <c r="L38" t="n">
-        <v>8.8390243902439</v>
+        <v>37</v>
       </c>
       <c r="M38" t="n">
-        <v>37</v>
-      </c>
-      <c r="N38" t="s">
-        <v>54</v>
+        <v>189.2</v>
+      </c>
+      <c r="N38" t="n">
+        <v>11</v>
       </c>
       <c r="O38" t="n">
-        <v>189.2</v>
+        <v>2.76780487804878</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0.88390243902439</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>76.4087804878049</v>
+      </c>
+      <c r="R38" t="n">
+        <v>22.9226341463415</v>
+      </c>
+      <c r="S38" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="39">
@@ -2335,10 +2803,10 @@
         <v>0.8</v>
       </c>
       <c r="C39" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D39" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E39" t="n">
         <v>1</v>
@@ -2353,25 +2821,37 @@
         <v>78</v>
       </c>
       <c r="I39" t="n">
-        <v>107.776</v>
+        <v>38.174358974359</v>
       </c>
       <c r="J39" t="n">
         <v>38.174358974359</v>
       </c>
       <c r="K39" t="n">
-        <v>38.174358974359</v>
+        <v>19.0871794871795</v>
       </c>
       <c r="L39" t="n">
-        <v>19.0871794871795</v>
+        <v>38</v>
       </c>
       <c r="M39" t="n">
-        <v>38</v>
-      </c>
-      <c r="N39" t="s">
-        <v>55</v>
+        <v>1250.8</v>
+      </c>
+      <c r="N39" t="n">
+        <v>23</v>
       </c>
       <c r="O39" t="n">
-        <v>1250.8</v>
+        <v>4.8174358974359</v>
+      </c>
+      <c r="P39" t="n">
+        <v>1.90871794871795</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>303.581538461539</v>
+      </c>
+      <c r="R39" t="n">
+        <v>91.0744615384615</v>
+      </c>
+      <c r="S39" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="40">
@@ -2382,10 +2862,10 @@
         <v>0.8</v>
       </c>
       <c r="C40" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D40" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E40" t="n">
         <v>10</v>
@@ -2400,25 +2880,37 @@
         <v>179</v>
       </c>
       <c r="I40" t="n">
-        <v>1934.024</v>
+        <v>80.4603351955307</v>
       </c>
       <c r="J40" t="n">
         <v>80.4603351955307</v>
       </c>
       <c r="K40" t="n">
-        <v>80.4603351955307</v>
+        <v>40.2301675977654</v>
       </c>
       <c r="L40" t="n">
-        <v>40.2301675977654</v>
+        <v>39</v>
       </c>
       <c r="M40" t="n">
-        <v>39</v>
-      </c>
-      <c r="N40" t="s">
-        <v>56</v>
+        <v>4242</v>
+      </c>
+      <c r="N40" t="n">
+        <v>53</v>
       </c>
       <c r="O40" t="n">
-        <v>4242</v>
+        <v>18.0460335195531</v>
+      </c>
+      <c r="P40" t="n">
+        <v>4.02301675977654</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>1889.77966480447</v>
+      </c>
+      <c r="R40" t="n">
+        <v>566.933899441341</v>
+      </c>
+      <c r="S40" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="41">
@@ -2429,10 +2921,10 @@
         <v>0.8</v>
       </c>
       <c r="C41" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D41" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E41" t="n">
         <v>10</v>
@@ -2447,25 +2939,37 @@
         <v>409</v>
       </c>
       <c r="I41" t="n">
-        <v>5026.016</v>
+        <v>228.854767726161</v>
       </c>
       <c r="J41" t="n">
         <v>228.854767726161</v>
       </c>
       <c r="K41" t="n">
-        <v>228.854767726161</v>
+        <v>114.427383863081</v>
       </c>
       <c r="L41" t="n">
-        <v>114.427383863081</v>
+        <v>40</v>
       </c>
       <c r="M41" t="n">
-        <v>40</v>
-      </c>
-      <c r="N41" t="s">
-        <v>57</v>
+        <v>23847.65</v>
+      </c>
+      <c r="N41" t="n">
+        <v>122</v>
       </c>
       <c r="O41" t="n">
-        <v>23847.65</v>
+        <v>32.8854767726161</v>
+      </c>
+      <c r="P41" t="n">
+        <v>11.4427383863081</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>10088.1222493888</v>
+      </c>
+      <c r="R41" t="n">
+        <v>3026.43667481663</v>
+      </c>
+      <c r="S41" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="42">
@@ -2473,13 +2977,13 @@
         <v>30</v>
       </c>
       <c r="B42" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C42" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D42" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E42" t="n">
         <v>1</v>
@@ -2488,31 +2992,43 @@
         <v>0.1</v>
       </c>
       <c r="G42" t="n">
-        <v>906</v>
+        <v>634.2</v>
       </c>
       <c r="H42" t="n">
         <v>41</v>
       </c>
       <c r="I42" t="n">
-        <v>59.12</v>
+        <v>15.4682926829268</v>
       </c>
       <c r="J42" t="n">
-        <v>22.0975609756098</v>
+        <v>15.4682926829268</v>
       </c>
       <c r="K42" t="n">
-        <v>22.0975609756098</v>
+        <v>7.73414634146341</v>
       </c>
       <c r="L42" t="n">
-        <v>11.0487804878049</v>
+        <v>41</v>
       </c>
       <c r="M42" t="n">
-        <v>41</v>
-      </c>
-      <c r="N42" t="s">
-        <v>58</v>
+        <v>189.2</v>
+      </c>
+      <c r="N42" t="n">
+        <v>11</v>
       </c>
       <c r="O42" t="n">
-        <v>189.2</v>
+        <v>2.54682926829268</v>
+      </c>
+      <c r="P42" t="n">
+        <v>0.773414634146341</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>68.2326829268293</v>
+      </c>
+      <c r="R42" t="n">
+        <v>34.1163414634146</v>
+      </c>
+      <c r="S42" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="43">
@@ -2520,13 +3036,13 @@
         <v>57</v>
       </c>
       <c r="B43" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C43" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D43" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E43" t="n">
         <v>1</v>
@@ -2535,31 +3051,43 @@
         <v>0.1</v>
       </c>
       <c r="G43" t="n">
-        <v>3722</v>
+        <v>2605.4</v>
       </c>
       <c r="H43" t="n">
         <v>78</v>
       </c>
       <c r="I43" t="n">
-        <v>152.44</v>
+        <v>33.4025641025641</v>
       </c>
       <c r="J43" t="n">
-        <v>47.7179487179487</v>
+        <v>33.4025641025641</v>
       </c>
       <c r="K43" t="n">
-        <v>47.7179487179487</v>
+        <v>16.701282051282</v>
       </c>
       <c r="L43" t="n">
-        <v>23.8589743589744</v>
+        <v>42</v>
       </c>
       <c r="M43" t="n">
-        <v>42</v>
-      </c>
-      <c r="N43" t="s">
-        <v>59</v>
+        <v>1250.8</v>
+      </c>
+      <c r="N43" t="n">
+        <v>23</v>
       </c>
       <c r="O43" t="n">
-        <v>1250.8</v>
+        <v>4.34025641025641</v>
+      </c>
+      <c r="P43" t="n">
+        <v>1.67012820512821</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>268.508846153846</v>
+      </c>
+      <c r="R43" t="n">
+        <v>134.254423076923</v>
+      </c>
+      <c r="S43" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="44">
@@ -2567,13 +3095,13 @@
         <v>118</v>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C44" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E44" t="n">
         <v>10</v>
@@ -2582,31 +3110,43 @@
         <v>0.1</v>
       </c>
       <c r="G44" t="n">
-        <v>18003</v>
+        <v>12602.1</v>
       </c>
       <c r="H44" t="n">
         <v>179</v>
       </c>
       <c r="I44" t="n">
-        <v>2150.06</v>
+        <v>70.4027932960894</v>
       </c>
       <c r="J44" t="n">
-        <v>100.575418994413</v>
+        <v>70.4027932960894</v>
       </c>
       <c r="K44" t="n">
-        <v>100.575418994413</v>
+        <v>35.2013966480447</v>
       </c>
       <c r="L44" t="n">
-        <v>50.2877094972067</v>
+        <v>43</v>
       </c>
       <c r="M44" t="n">
-        <v>43</v>
-      </c>
-      <c r="N44" t="s">
-        <v>60</v>
+        <v>4242</v>
+      </c>
+      <c r="N44" t="n">
+        <v>53</v>
       </c>
       <c r="O44" t="n">
-        <v>4242</v>
+        <v>17.0402793296089</v>
+      </c>
+      <c r="P44" t="n">
+        <v>3.52013966480447</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>1719.80720670391</v>
+      </c>
+      <c r="R44" t="n">
+        <v>859.903603351955</v>
+      </c>
+      <c r="S44" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="45">
@@ -2614,13 +3154,13 @@
         <v>300</v>
       </c>
       <c r="B45" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C45" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D45" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E45" t="n">
         <v>10</v>
@@ -2629,31 +3169,43 @@
         <v>0.1</v>
       </c>
       <c r="G45" t="n">
-        <v>117002</v>
+        <v>81901.4</v>
       </c>
       <c r="H45" t="n">
         <v>409</v>
       </c>
       <c r="I45" t="n">
-        <v>6430.04</v>
+        <v>200.247921760391</v>
       </c>
       <c r="J45" t="n">
-        <v>286.068459657702</v>
+        <v>200.247921760391</v>
       </c>
       <c r="K45" t="n">
-        <v>286.068459657702</v>
+        <v>100.123960880196</v>
       </c>
       <c r="L45" t="n">
-        <v>143.034229828851</v>
+        <v>44</v>
       </c>
       <c r="M45" t="n">
-        <v>44</v>
-      </c>
-      <c r="N45" t="s">
-        <v>61</v>
+        <v>23847.65</v>
+      </c>
+      <c r="N45" t="n">
+        <v>122</v>
       </c>
       <c r="O45" t="n">
-        <v>23847.65</v>
+        <v>30.0247921760391</v>
+      </c>
+      <c r="P45" t="n">
+        <v>10.0123960880196</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>8979.60696821516</v>
+      </c>
+      <c r="R45" t="n">
+        <v>4489.80348410758</v>
+      </c>
+      <c r="S45" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="46">
@@ -2664,10 +3216,10 @@
         <v>0.8</v>
       </c>
       <c r="C46" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D46" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E46" t="n">
         <v>1</v>
@@ -2682,25 +3234,37 @@
         <v>41</v>
       </c>
       <c r="I46" t="n">
-        <v>55.496</v>
+        <v>17.6780487804878</v>
       </c>
       <c r="J46" t="n">
         <v>17.6780487804878</v>
       </c>
       <c r="K46" t="n">
-        <v>17.6780487804878</v>
+        <v>8.8390243902439</v>
       </c>
       <c r="L46" t="n">
-        <v>8.8390243902439</v>
+        <v>45</v>
       </c>
       <c r="M46" t="n">
-        <v>45</v>
-      </c>
-      <c r="N46" t="s">
-        <v>62</v>
+        <v>189.2</v>
+      </c>
+      <c r="N46" t="n">
+        <v>11</v>
       </c>
       <c r="O46" t="n">
-        <v>189.2</v>
+        <v>2.76780487804878</v>
+      </c>
+      <c r="P46" t="n">
+        <v>0.88390243902439</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>76.4087804878049</v>
+      </c>
+      <c r="R46" t="n">
+        <v>38.2043902439024</v>
+      </c>
+      <c r="S46" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="47">
@@ -2711,10 +3275,10 @@
         <v>0.8</v>
       </c>
       <c r="C47" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D47" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E47" t="n">
         <v>1</v>
@@ -2729,25 +3293,37 @@
         <v>78</v>
       </c>
       <c r="I47" t="n">
-        <v>137.552</v>
+        <v>38.174358974359</v>
       </c>
       <c r="J47" t="n">
         <v>38.174358974359</v>
       </c>
       <c r="K47" t="n">
-        <v>38.174358974359</v>
+        <v>19.0871794871795</v>
       </c>
       <c r="L47" t="n">
-        <v>19.0871794871795</v>
+        <v>46</v>
       </c>
       <c r="M47" t="n">
-        <v>46</v>
-      </c>
-      <c r="N47" t="s">
-        <v>63</v>
+        <v>1250.8</v>
+      </c>
+      <c r="N47" t="n">
+        <v>23</v>
       </c>
       <c r="O47" t="n">
-        <v>1250.8</v>
+        <v>4.8174358974359</v>
+      </c>
+      <c r="P47" t="n">
+        <v>1.90871794871795</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>303.581538461539</v>
+      </c>
+      <c r="R47" t="n">
+        <v>151.790769230769</v>
+      </c>
+      <c r="S47" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="48">
@@ -2758,10 +3334,10 @@
         <v>0.8</v>
       </c>
       <c r="C48" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D48" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E48" t="n">
         <v>10</v>
@@ -2776,25 +3352,37 @@
         <v>179</v>
       </c>
       <c r="I48" t="n">
-        <v>2078.048</v>
+        <v>80.4603351955307</v>
       </c>
       <c r="J48" t="n">
         <v>80.4603351955307</v>
       </c>
       <c r="K48" t="n">
-        <v>80.4603351955307</v>
+        <v>40.2301675977654</v>
       </c>
       <c r="L48" t="n">
-        <v>40.2301675977654</v>
+        <v>47</v>
       </c>
       <c r="M48" t="n">
-        <v>47</v>
-      </c>
-      <c r="N48" t="s">
-        <v>64</v>
+        <v>4242</v>
+      </c>
+      <c r="N48" t="n">
+        <v>53</v>
       </c>
       <c r="O48" t="n">
-        <v>4242</v>
+        <v>18.0460335195531</v>
+      </c>
+      <c r="P48" t="n">
+        <v>4.02301675977654</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>1889.77966480447</v>
+      </c>
+      <c r="R48" t="n">
+        <v>944.889832402235</v>
+      </c>
+      <c r="S48" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="49">
@@ -2805,10 +3393,10 @@
         <v>0.8</v>
       </c>
       <c r="C49" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D49" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E49" t="n">
         <v>10</v>
@@ -2823,25 +3411,37 @@
         <v>409</v>
       </c>
       <c r="I49" t="n">
-        <v>5962.032</v>
+        <v>228.854767726161</v>
       </c>
       <c r="J49" t="n">
         <v>228.854767726161</v>
       </c>
       <c r="K49" t="n">
-        <v>228.854767726161</v>
+        <v>114.427383863081</v>
       </c>
       <c r="L49" t="n">
-        <v>114.427383863081</v>
+        <v>48</v>
       </c>
       <c r="M49" t="n">
-        <v>48</v>
-      </c>
-      <c r="N49" t="s">
-        <v>65</v>
+        <v>23847.65</v>
+      </c>
+      <c r="N49" t="n">
+        <v>122</v>
       </c>
       <c r="O49" t="n">
-        <v>23847.65</v>
+        <v>32.8854767726161</v>
+      </c>
+      <c r="P49" t="n">
+        <v>11.4427383863081</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>10088.1222493888</v>
+      </c>
+      <c r="R49" t="n">
+        <v>5044.06112469438</v>
+      </c>
+      <c r="S49" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Batch parameters for new budget parameters
</commit_message>
<xml_diff>
--- a/analysis/new.batch.parameters.xlsx
+++ b/analysis/new.batch.parameters.xlsx
@@ -122,55 +122,55 @@
     <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance300 --budget 5044.06112469438 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 16</t>
   </si>
   <si>
-    <t xml:space="preserve">main_program.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance30 --budget 20.4698048780488 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance57 --budget 80.5526538461538 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance118 --budget 515.942162011173 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance300 --budget 2693.88209046455 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance30 --budget 22.9226341463415 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance57 --budget 91.0744615384615 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance118 --budget 566.933899441341 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance300 --budget 3026.43667481663 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance30 --budget 34.1163414634146 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance57 --budget 134.254423076923 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance118 --budget 859.903603351955 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance300 --budget 4489.80348410758 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance30 --budget 38.2043902439024 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance57 --budget 151.790769230769 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance118 --budget 944.889832402235 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --instance_location instance300 --budget 5044.06112469438 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 32</t>
+    <t xml:space="preserve">main_program.py --mip_emphasis 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance30 --budget 20.4698048780488 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance57 --budget 80.5526538461538 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance118 --budget 515.942162011173 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance300 --budget 2693.88209046455 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance30 --budget 22.9226341463415 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance57 --budget 91.0744615384615 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance118 --budget 566.933899441341 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance300 --budget 3026.43667481663 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance30 --budget 34.1163414634146 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance57 --budget 134.254423076923 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance118 --budget 859.903603351955 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance300 --budget 4489.80348410758 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance30 --budget 38.2043902439024 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance57 --budget 151.790769230769 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance118 --budget 944.889832402235 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance300 --budget 5044.06112469438 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 32</t>
   </si>
   <si>
     <t xml:space="preserve">main_program_one_depth_cascade.py</t>

</xml_diff>

<commit_message>
Modified run parameters for 12 hours + export of instance results. Batch file also updated.
</commit_message>
<xml_diff>
--- a/analysis/new.batch.parameters.xlsx
+++ b/analysis/new.batch.parameters.xlsx
@@ -122,106 +122,106 @@
     <t xml:space="preserve">python robustness_heuristic_upper_bound.py --instance_location instance300 --budget 5044.06112469438 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 16</t>
   </si>
   <si>
-    <t xml:space="preserve">main_program.py --mip_emphasis 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance30 --budget 20.4698048780488 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance57 --budget 80.5526538461538 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance118 --budget 515.942162011173 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance300 --budget 2693.88209046455 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance30 --budget 22.9226341463415 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance57 --budget 91.0744615384615 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance118 --budget 566.933899441341 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance300 --budget 3026.43667481663 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance30 --budget 34.1163414634146 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance57 --budget 134.254423076923 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance118 --budget 859.903603351955 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance300 --budget 4489.80348410758 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance30 --budget 38.2043902439024 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance57 --budget 151.790769230769 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance118 --budget 944.889832402235 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --instance_location instance300 --budget 5044.06112469438 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">main_program_one_depth_cascade.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance30 --budget 20.4698048780488 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance57 --budget 80.5526538461538 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance118 --budget 515.942162011173 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance300 --budget 2693.88209046455 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance30 --budget 22.9226341463415 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance57 --budget 91.0744615384615 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance118 --budget 566.933899441341 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance300 --budget 3026.43667481663 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance30 --budget 34.1163414634146 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance57 --budget 134.254423076923 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance118 --budget 859.903603351955 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance300 --budget 4489.80348410758 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance30 --budget 38.2043902439024 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance57 --budget 151.790769230769 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance118 --budget 944.889832402235 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">python main_program_one_depth_cascade.py --instance_location instance300 --budget 5044.06112469438 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 48</t>
+    <t xml:space="preserve">main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file --instance_location instance30 --budget 20.4698048780488 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file --instance_location instance57 --budget 80.5526538461538 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file --instance_location instance118 --budget 515.942162011173 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file --instance_location instance300 --budget 2693.88209046455 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file --instance_location instance30 --budget 22.9226341463415 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file --instance_location instance57 --budget 91.0744615384615 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file --instance_location instance118 --budget 566.933899441341 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file --instance_location instance300 --budget 3026.43667481663 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file --instance_location instance30 --budget 34.1163414634146 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file --instance_location instance57 --budget 134.254423076923 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file --instance_location instance118 --budget 859.903603351955 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file --instance_location instance300 --budget 4489.80348410758 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file --instance_location instance30 --budget 38.2043902439024 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file --instance_location instance57 --budget 151.790769230769 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file --instance_location instance118 --budget 944.889832402235 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program.py --mip_emphasis 1 --timelimit 12 --export_results_file --instance_location instance300 --budget 5044.06112469438 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">main_program_one_depth_cascade.py --timelimit 12 --export_results_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --timelimit 12 --export_results_file --instance_location instance30 --budget 20.4698048780488 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --timelimit 12 --export_results_file --instance_location instance57 --budget 80.5526538461538 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --timelimit 12 --export_results_file --instance_location instance118 --budget 515.942162011173 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --timelimit 12 --export_results_file --instance_location instance300 --budget 2693.88209046455 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --timelimit 12 --export_results_file --instance_location instance30 --budget 22.9226341463415 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --timelimit 12 --export_results_file --instance_location instance57 --budget 91.0744615384615 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --timelimit 12 --export_results_file --instance_location instance118 --budget 566.933899441341 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --timelimit 12 --export_results_file --instance_location instance300 --budget 3026.43667481663 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --timelimit 12 --export_results_file --instance_location instance30 --budget 34.1163414634146 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 7.73414634146341 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 15.4682926829268 --dump_file 41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --timelimit 12 --export_results_file --instance_location instance57 --budget 134.254423076923 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 16.701282051282 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 33.4025641025641 --dump_file 42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --timelimit 12 --export_results_file --instance_location instance118 --budget 859.903603351955 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 35.2013966480447 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 70.4027932960894 --dump_file 43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --timelimit 12 --export_results_file --instance_location instance300 --budget 4489.80348410758 --load_capacity_factor 0.7 --line_upgrade_capacity_coef_scale 100.123960880196 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 200.247921760391 --dump_file 44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --timelimit 12 --export_results_file --instance_location instance30 --budget 38.2043902439024 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 8.8390243902439 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 17.6780487804878 --dump_file 45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --timelimit 12 --export_results_file --instance_location instance57 --budget 151.790769230769 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 19.0871794871795 --line_establish_cost_coef_scale 1 --line_establish_capacity_coef_scale 38.174358974359 --dump_file 46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --timelimit 12 --export_results_file --instance_location instance118 --budget 944.889832402235 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 40.2301675977654 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 80.4603351955307 --dump_file 47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python main_program_one_depth_cascade.py --timelimit 12 --export_results_file --instance_location instance300 --budget 5044.06112469438 --load_capacity_factor 0.8 --line_upgrade_capacity_coef_scale 114.427383863081 --line_establish_cost_coef_scale 10 --line_establish_capacity_coef_scale 228.854767726161 --dump_file 48</t>
   </si>
 </sst>
 </file>

</xml_diff>